<commit_message>
Removed Encounter.header data, keep order in mapped tables
</commit_message>
<xml_diff>
--- a/maps/Encounter.xlsx
+++ b/maps/Encounter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Nictiz\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FC1B65-8413-4AF5-84EA-2339A68C520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40490518-20AA-47AF-A604-EDBE625C23C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13500" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{02FC4626-A12F-4F2B-A4F9-C91521D9ECCA}"/>
+    <workbookView xWindow="-1365" yWindow="-17340" windowWidth="38700" windowHeight="15345" xr2:uid="{02FC4626-A12F-4F2B-A4F9-C91521D9ECCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>xtehr</t>
   </si>
@@ -48,39 +48,6 @@
   </si>
   <si>
     <t>EHDSEncounter.header</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.subject</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.identifier</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.authorship</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.authorship.author[x]</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.authorship.datetime</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.lastUpdate</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.status</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.statusReason[x]</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.language</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.header.version</t>
-  </si>
-  <si>
-    <t>EHDSEncounter.presentedForm</t>
   </si>
   <si>
     <t>EHDSEncounter.priority</t>
@@ -578,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8631DB2A-343D-442B-A304-5E36E8950659}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD60"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,6 +587,9 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -642,211 +612,153 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
+      <c r="B10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
+      <c r="B19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
+      <c r="B25" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>25</v>
+      <c r="B26" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
+      <c r="B27" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>42</v>
+      <c r="A30" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>44</v>
+      <c r="A32" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>45</v>
+      <c r="A33" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>46</v>
+      <c r="A34" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>47</v>
+      <c r="A35" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>